<commit_message>
Annotative lines. Manual bubble organization.
</commit_message>
<xml_diff>
--- a/BubbleVelocity_Manually.xlsx
+++ b/BubbleVelocity_Manually.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wongb\Documents\Python_Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C1B7E7-A94B-47BF-A422-EE6555D1DF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC9A1E8-B3C5-46D5-BD5D-3761E39A3AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="24" windowWidth="16632" windowHeight="11076" xr2:uid="{EE926819-E7B1-4DC3-8767-F7968B0932F0}"/>
+    <workbookView xWindow="864" yWindow="1260" windowWidth="16632" windowHeight="11076" activeTab="1" xr2:uid="{EE926819-E7B1-4DC3-8767-F7968B0932F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>X</t>
   </si>
@@ -109,6 +110,15 @@
   </si>
   <si>
     <t>avg acceleration</t>
+  </si>
+  <si>
+    <t>cm/Myr</t>
+  </si>
+  <si>
+    <t>multiply by</t>
+  </si>
+  <si>
+    <t>(31536*10^9)^-1</t>
   </si>
 </sst>
 </file>
@@ -116,7 +126,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -151,7 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B68814B-175C-4FA3-97EA-F61A09615228}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,9 +672,15 @@
         <v>12</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -677,9 +693,17 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="D10" s="3">
+        <f>(C8-C7)</f>
+        <v>-5.2128999999999993E+20</v>
+      </c>
+      <c r="E10" s="3">
+        <f>(C8-C7)/10</f>
+        <v>-5.2128999999999992E+19</v>
+      </c>
+      <c r="F10" s="3">
+        <v>-1653000</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1116,6 +1140,12 @@
         <f t="shared" si="0"/>
         <v>5.4337999999999984E+19</v>
       </c>
+      <c r="F35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>20</v>
+      </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
@@ -1135,6 +1165,12 @@
       <c r="E36" s="3">
         <f t="shared" si="0"/>
         <v>2.442100000000002E+19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" t="s">
+        <v>27</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -1148,7 +1184,7 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>18</v>
@@ -1177,13 +1213,13 @@
         <v>6.9714714285714293E+19</v>
       </c>
       <c r="G38" s="3">
-        <v>70000000</v>
+        <v>700000000</v>
       </c>
       <c r="H38" s="3">
-        <v>7000000000000</v>
+        <v>70000000000000</v>
       </c>
       <c r="I38" s="3">
-        <v>220000</v>
+        <v>2200000</v>
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -1326,4 +1362,351 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43FD566-B5B0-478D-8761-0B23F62199D3}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="6" max="8" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>75</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>76</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2.3095299999999998E+22</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-9.8483999999999995E+21</v>
+      </c>
+      <c r="E4">
+        <v>76</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>77</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="E5">
+        <v>77</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>78</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="E6">
+        <v>78</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2.3259300000000001E+22</v>
+      </c>
+      <c r="G6" s="3">
+        <v>-7.8329400000000001E+21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>79</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2.32173E+22</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-8.8039099999999995E+21</v>
+      </c>
+      <c r="E7">
+        <v>79</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.3236200000000002E+22</v>
+      </c>
+      <c r="G7" s="3">
+        <v>-7.4072900000000005E+21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>80</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2.32275E+22</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-9.3251999999999995E+21</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2.3208700000000002E+22</v>
+      </c>
+      <c r="G8" s="3">
+        <v>-6.5714400000000005E+21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>81</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="E9">
+        <v>81</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.3282799999999998E+22</v>
+      </c>
+      <c r="G9" s="3">
+        <v>-5.5463400000000004E+21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>82</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="E10">
+        <v>82</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2.3257300000000002E+22</v>
+      </c>
+      <c r="G10" s="3">
+        <v>-5.0166000000000003E+21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>83</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="E11">
+        <v>83</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2.3242000000000002E+22</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-3.7404999999999999E+21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>84</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="E12">
+        <v>84</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2.3276000000000001E+22</v>
+      </c>
+      <c r="G12" s="3">
+        <v>-3.19712E+21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>85</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="E13">
+        <v>85</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2.3270100000000002E+22</v>
+      </c>
+      <c r="G13" s="3">
+        <v>-2.9529099999999998E+21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>86</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="E14">
+        <v>86</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>87</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="E15">
+        <v>87</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>88</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="E16">
+        <v>88</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>89</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="E17">
+        <v>89</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>90</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="E18">
+        <v>90</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>91</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="E19">
+        <v>91</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>92</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="E20">
+        <v>92</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>93</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="E21">
+        <v>93</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>94</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="E22">
+        <v>94</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>95</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="E23">
+        <v>95</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started using velocity estimation, added .csv output capability
</commit_message>
<xml_diff>
--- a/BubbleVelocity_Manually.xlsx
+++ b/BubbleVelocity_Manually.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wongb\Documents\Python_Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BD9C84-8BB0-4CDB-826A-FB2014F848B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4953D20B-7C3F-436F-B8D3-B6F9A37CAB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="864" yWindow="1260" windowWidth="16632" windowHeight="11076" activeTab="1" xr2:uid="{EE926819-E7B1-4DC3-8767-F7968B0932F0}"/>
+    <workbookView xWindow="3000" yWindow="1248" windowWidth="12564" windowHeight="11076" activeTab="1" xr2:uid="{EE926819-E7B1-4DC3-8767-F7968B0932F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>X</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>(31536*10^9)^-1</t>
+  </si>
+  <si>
+    <t>bad code/border</t>
+  </si>
+  <si>
+    <t>velocity in cm/s</t>
+  </si>
+  <si>
+    <t>10Myr--&gt;S</t>
+  </si>
+  <si>
+    <t>1/(525600*60E+7)</t>
   </si>
 </sst>
 </file>
@@ -157,16 +169,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -478,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B68814B-175C-4FA3-97EA-F61A09615228}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:C46"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43FD566-B5B0-478D-8761-0B23F62199D3}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1378,15 +1452,24 @@
     <col min="6" max="8" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1">
+        <v>3.1709791999999999E-15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1405,212 +1488,286 @@
       <c r="G2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>75</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="3">
+        <v>2.2871316E+22</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-9.8885268400000006E+21</v>
+      </c>
       <c r="E3">
         <v>75</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>76</v>
       </c>
       <c r="B4" s="3">
-        <v>2.3095299999999998E+22</v>
+        <v>2.2871316E+22</v>
       </c>
       <c r="C4" s="3">
-        <v>-9.8483999999999995E+21</v>
+        <v>-1.0163973399999999E+22</v>
+      </c>
+      <c r="D4" s="3">
+        <f>(C4-C3)*$I$1</f>
+        <v>-873435.31247154821</v>
       </c>
       <c r="E4">
         <v>76</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>77</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="3">
+        <v>2.2871316E+22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-1.0604687999999999E+22</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D9" si="0">(C5-C4)*$I$1</f>
+        <v>-1397496.8297363203</v>
+      </c>
       <c r="E5">
         <v>77</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>78</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3"/>
+      <c r="B6" s="3">
+        <v>2.2871316E+22</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-1.1045401399999999E+22</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>-1397493.0245612792</v>
+      </c>
       <c r="E6">
         <v>78</v>
       </c>
       <c r="F6" s="3">
-        <v>2.3259300000000001E+22</v>
-      </c>
-      <c r="G6" s="3">
-        <v>-7.8329400000000001E+21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2.2871316E+22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>79</v>
       </c>
       <c r="B7" s="3">
-        <v>2.32173E+22</v>
+        <v>2.2871316E+22</v>
       </c>
       <c r="C7" s="3">
-        <v>-8.8039099999999995E+21</v>
-      </c>
+        <v>-8.8418303700000005E+21</v>
+      </c>
+      <c r="D7" s="3"/>
       <c r="E7">
         <v>79</v>
       </c>
       <c r="F7" s="3">
-        <v>2.3236200000000002E+22</v>
-      </c>
-      <c r="G7" s="3">
-        <v>-7.4072900000000005E+21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2.2871316E+22</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>80</v>
       </c>
       <c r="B8" s="3">
-        <v>2.32275E+22</v>
+        <v>2.2871316E+22</v>
       </c>
       <c r="C8" s="3">
         <v>-9.3251999999999995E+21</v>
       </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>-1532755.0426416926</v>
+      </c>
       <c r="E8">
         <v>80</v>
       </c>
       <c r="F8" s="3">
-        <v>2.3208700000000002E+22</v>
+        <v>2.2871316E+22</v>
       </c>
       <c r="G8" s="3">
-        <v>-6.5714400000000005E+21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-6.5280801699999997E+21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>81</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3">
+        <v>2.2871316E+22</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-5.5915623400000004E+21</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>11839287.360196669</v>
+      </c>
       <c r="E9">
         <v>81</v>
       </c>
       <c r="F9" s="3">
-        <v>2.3282799999999998E+22</v>
+        <v>2.2871316E+22</v>
       </c>
       <c r="G9" s="3">
-        <v>-5.5463400000000004E+21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-4.04906258E+21</v>
+      </c>
+      <c r="H9" s="3">
+        <f>(G9-G8)*$I$1</f>
+        <v>7860913.214324127</v>
+      </c>
+      <c r="I9" s="4" t="e">
+        <f>H9*H1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>82</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="E10">
         <v>82</v>
       </c>
       <c r="F10" s="3">
-        <v>2.3257300000000002E+22</v>
+        <v>2.2871316E+22</v>
       </c>
       <c r="G10" s="3">
-        <v>-5.0166000000000003E+21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-4.9855804100000004E+21</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" ref="H10:H12" si="1">(G10-G9)*$I$1</f>
+        <v>-2969678.559359137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>83</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="E11">
         <v>83</v>
       </c>
       <c r="F11" s="3">
-        <v>2.3242000000000002E+22</v>
+        <v>2.2871316E+22</v>
       </c>
       <c r="G11" s="3">
-        <v>-3.7404999999999999E+21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-4.0490622899999998E+21</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="1"/>
+        <v>2969679.4789431058</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>84</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="E12">
         <v>84</v>
       </c>
       <c r="F12" s="3">
-        <v>2.3276000000000001E+22</v>
+        <v>2.2871316E+22</v>
       </c>
       <c r="G12" s="3">
-        <v>-3.19712E+21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-3.2227231000000001E+21</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="1"/>
+        <v>2620304.3836348467</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>85</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="E13">
         <v>85</v>
       </c>
       <c r="F13" s="3">
-        <v>2.3270100000000002E+22</v>
-      </c>
-      <c r="G13" s="3">
-        <v>-2.9529099999999998E+21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2.2871316E+22</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>86</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="E14">
         <v>86</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>87</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="E15">
         <v>87</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>88</v>
       </c>
@@ -1619,7 +1776,9 @@
       <c r="E16">
         <v>88</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1631,7 +1790,9 @@
       <c r="E17">
         <v>89</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1643,7 +1804,9 @@
       <c r="E18">
         <v>90</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1655,7 +1818,9 @@
       <c r="E19">
         <v>91</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3">
+        <v>2.2871316E+22</v>
+      </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1707,6 +1872,19 @@
       <c r="G23" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C3:C6">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>-9E+99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:C9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>-9E+99</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Validating LHS equation; fixed ypos error on G9
</commit_message>
<xml_diff>
--- a/BubbleVelocity_Manually.xlsx
+++ b/BubbleVelocity_Manually.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wongb\Documents\Python_Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4953D20B-7C3F-436F-B8D3-B6F9A37CAB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923C8506-F87B-44EC-9C03-5FE412822428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1248" windowWidth="12564" windowHeight="11076" activeTab="1" xr2:uid="{EE926819-E7B1-4DC3-8767-F7968B0932F0}"/>
+    <workbookView xWindow="-72" yWindow="3564" windowWidth="15540" windowHeight="9228" activeTab="1" xr2:uid="{EE926819-E7B1-4DC3-8767-F7968B0932F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -187,36 +187,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1442,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43FD566-B5B0-478D-8761-0B23F62199D3}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1642,11 +1612,11 @@
         <v>2.2871316E+22</v>
       </c>
       <c r="G9" s="3">
-        <v>-4.04906258E+21</v>
+        <v>-5.5915640000000001E+21</v>
       </c>
       <c r="H9" s="3">
         <f>(G9-G8)*$I$1</f>
-        <v>7860913.214324127</v>
+        <v>2969673.2955336627</v>
       </c>
       <c r="I9" s="4" t="e">
         <f>H9*H1</f>
@@ -1672,7 +1642,7 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" ref="H10:H12" si="1">(G10-G9)*$I$1</f>
-        <v>-2969678.559359137</v>
+        <v>1921561.3594313271</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1873,10 +1843,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>-9E+99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed some bubble y data points, polished LHS code
</commit_message>
<xml_diff>
--- a/BubbleVelocity_Manually.xlsx
+++ b/BubbleVelocity_Manually.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wongb\Documents\Python_Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDA7F0E-CB7A-4E83-94EA-ABF84EB48D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EE1488-4EC1-4A7E-AEF6-E46B6362401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="3684" windowWidth="15540" windowHeight="9228" activeTab="1" xr2:uid="{EE926819-E7B1-4DC3-8767-F7968B0932F0}"/>
+    <workbookView xWindow="7476" yWindow="96" windowWidth="15540" windowHeight="9228" activeTab="1" xr2:uid="{EE926819-E7B1-4DC3-8767-F7968B0932F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>X</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>1/(525600*60E+7)</t>
+  </si>
+  <si>
+    <t>upper upper</t>
   </si>
 </sst>
 </file>
@@ -149,12 +152,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,17 +178,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1410,19 +1450,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43FD566-B5B0-478D-8761-0B23F62199D3}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="15.77734375" customWidth="1"/>
     <col min="6" max="8" width="15.77734375" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1439,7 +1481,7 @@
         <v>3.1709791999999999E-15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1462,7 +1504,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>75</v>
       </c>
@@ -1480,7 +1522,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>76</v>
       </c>
@@ -1502,7 +1544,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>77</v>
       </c>
@@ -1524,7 +1566,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>78</v>
       </c>
@@ -1545,7 +1587,7 @@
         <v>2.2871316E+22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>79</v>
       </c>
@@ -1566,8 +1608,11 @@
       <c r="H7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>80</v>
       </c>
@@ -1591,20 +1636,15 @@
         <v>-6.5280801699999997E+21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>81</v>
       </c>
       <c r="B9" s="3">
         <v>2.2871316E+22</v>
       </c>
-      <c r="C9" s="3">
-        <v>-5.5915623400000004E+21</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>11839287.360196669</v>
-      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3"/>
       <c r="E9">
         <v>81</v>
       </c>
@@ -1622,8 +1662,12 @@
         <f>H9*H1</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="1">
+        <v>-3.7185266699999998E+21</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>82</v>
       </c>
@@ -1644,8 +1688,15 @@
         <f t="shared" ref="H10:H12" si="1">(G10-G9)*$I$1</f>
         <v>1921561.3594313271</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="1">
+        <v>-3.7185266699999998E+21</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" ref="K10:K11" si="2">(J10-J9)*$I$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>83</v>
       </c>
@@ -1666,8 +1717,15 @@
         <f t="shared" si="1"/>
         <v>2969679.4789431058</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="1">
+        <v>-4.0490622899999998E+21</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="2"/>
+        <v>-1048121.5758791039</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>84</v>
       </c>
@@ -1689,7 +1747,7 @@
         <v>2620304.3836348467</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>85</v>
       </c>
@@ -1705,7 +1763,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>86</v>
       </c>
@@ -1721,7 +1779,7 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>87</v>
       </c>
@@ -1737,7 +1795,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>88</v>
       </c>
@@ -1843,18 +1901,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>-9E+99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C9">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="C7:C8">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>-9E+99</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>